<commit_message>
data excel file update
</commit_message>
<xml_diff>
--- a/bechdel_movie_data_20_25.xlsx
+++ b/bechdel_movie_data_20_25.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4925D523-D710-1740-AE56-311ED374CCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99110053-494A-354D-86D8-553041AD083B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13931,11 +13931,11 @@
     <t>Culpa Mía</t>
   </si>
   <si>
-    <t>original_tittle</t>
+    <t>original_title</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>primary_tittle</t>
+    <t>primary_title</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -14381,8 +14381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W864"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A826" zoomScale="106" workbookViewId="0">
-      <selection activeCell="P850" sqref="P850"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>

</xml_diff>